<commit_message>
updates: reliability & estimation calculations + exel
</commit_message>
<xml_diff>
--- a/static/exel_templates/report_template.xlsx
+++ b/static/exel_templates/report_template.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniil/Desktop/DIPLOM/evaluatingMaterialApp/static/exel_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F07F982-A1F3-8944-A169-6823749D377A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9778E8BC-67FF-5947-9FE9-BF1EE9014284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="500" windowWidth="31520" windowHeight="20500" xr2:uid="{EDD4186A-6E89-4516-944D-5EFD2E0820A6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="2" xr2:uid="{EDD4186A-6E89-4516-944D-5EFD2E0820A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Водозащита" sheetId="1" r:id="rId1"/>
     <sheet name="Гомеостаз" sheetId="2" r:id="rId2"/>
-    <sheet name="Надежность" sheetId="3" r:id="rId3"/>
+    <sheet name="Надежность" sheetId="5" r:id="rId3"/>
     <sheet name="Оценка" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -38,10 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="81">
-  <si>
-    <t>Оценка</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="104">
   <si>
     <t>Рп – давление промокания материалов</t>
   </si>
@@ -281,13 +278,85 @@
   </si>
   <si>
     <t>Sпр - площадь поверхности пробы:</t>
+  </si>
+  <si>
+    <t>Рпо – отрносительное давление промокания после нагрузок</t>
+  </si>
+  <si>
+    <t>Во – относительная водонепроницаемость после нагрузок</t>
+  </si>
+  <si>
+    <t>tпо – относительное время промокания материала после нагрузок</t>
+  </si>
+  <si>
+    <t>Кво – относителный критерий полноты реализации водозащитной функции после нагрузок</t>
+  </si>
+  <si>
+    <t>Рес – ресурс водозащитной функции материала</t>
+  </si>
+  <si>
+    <t>количество циклов воздействий</t>
+  </si>
+  <si>
+    <t>тип преобладающей нагрузки</t>
+  </si>
+  <si>
+    <t>параметры нагрузки</t>
+  </si>
+  <si>
+    <t>минимальная температура наружной среды</t>
+  </si>
+  <si>
+    <t>максимальная влажность наружной среды</t>
+  </si>
+  <si>
+    <t>ввод условия</t>
+  </si>
+  <si>
+    <t>выбор условия</t>
+  </si>
+  <si>
+    <t>циклов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">среднее арифметическое взвешенное </t>
+  </si>
+  <si>
+    <t>весомость функции водозащиты</t>
+  </si>
+  <si>
+    <t>весомость функции гомеостаза</t>
+  </si>
+  <si>
+    <t>весомость функции надежности</t>
+  </si>
+  <si>
+    <t>ввод</t>
+  </si>
+  <si>
+    <t xml:space="preserve">среднее геометрическое взвешенное </t>
+  </si>
+  <si>
+    <t>Изгиб</t>
+  </si>
+  <si>
+    <t>Истирание</t>
+  </si>
+  <si>
+    <t>Растяжение-сжатие</t>
+  </si>
+  <si>
+    <t>Кручение</t>
+  </si>
+  <si>
+    <t>Стирка</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,6 +395,12 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF9C5700"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -356,7 +431,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -600,6 +675,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -607,7 +713,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -708,6 +814,15 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -780,7 +895,39 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1100,8 +1247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90121C74-E08C-4AA5-AF53-2CE87386761F}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView zoomScale="93" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -1121,22 +1268,22 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1147,45 +1294,45 @@
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="62"/>
+      <c r="E5" s="5"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="52"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="55"/>
       <c r="F7" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="10" t="s">
-        <v>42</v>
-      </c>
       <c r="I7" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -1195,22 +1342,22 @@
         <v>ввод ЭД</v>
       </c>
       <c r="G8" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H8" s="26" t="e">
         <f>F8/G8</f>
         <v>#VALUE!</v>
       </c>
       <c r="I8" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1220,22 +1367,22 @@
         <v>ввод ЭД</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H9" s="26" t="e">
         <f t="shared" ref="H9:H10" si="0">F9/G9</f>
         <v>#VALUE!</v>
       </c>
       <c r="I9" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1245,25 +1392,25 @@
         <v>ввод ЭД</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H10" s="26" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="I10" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -1272,84 +1419,84 @@
         <v>#VALUE!</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H11" s="26" t="e">
         <f>F11/G11</f>
         <v>#VALUE!</v>
       </c>
       <c r="I11" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F12" s="35" t="e">
         <f>0.1*(4*B12+3*C12+2*D12+E12)/B16</f>
         <v>#VALUE!</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H12" s="26" t="e">
         <f>F12/G12</f>
         <v>#VALUE!</v>
       </c>
       <c r="I12" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="6"/>
     </row>
     <row r="14" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="14" t="s">
         <v>10</v>
-      </c>
-      <c r="B14" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1357,75 +1504,75 @@
       <c r="B17" s="6"/>
     </row>
     <row r="18" spans="1:9" ht="49" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="43"/>
+      <c r="A18" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="46"/>
       <c r="I18" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="39"/>
-      <c r="B19" s="44"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="46"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="49"/>
       <c r="I19" s="25" t="e">
         <f>((H8^I8)*(H9^I9)*(H10^I10)*(H11^I11)*(H12^I12))^(1/5)</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="39"/>
-      <c r="B20" s="44"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="46"/>
+      <c r="A20" s="42"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="49"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="39"/>
-      <c r="B21" s="44"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="46"/>
+      <c r="A21" s="42"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="49"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="39"/>
-      <c r="B22" s="44"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="45"/>
-      <c r="G22" s="45"/>
-      <c r="H22" s="46"/>
+      <c r="A22" s="42"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="49"/>
     </row>
     <row r="23" spans="1:9" ht="49" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="40"/>
-      <c r="B23" s="47"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="49"/>
+      <c r="A23" s="43"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="52"/>
     </row>
     <row r="24" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1433,12 +1580,12 @@
     </row>
     <row r="26" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1456,8 +1603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA1B50F2-689A-48B0-86F9-2E2A4FD4E6ED}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="81" zoomScaleNormal="119" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView zoomScale="81" zoomScaleNormal="119" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -1477,85 +1624,85 @@
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="19"/>
     </row>
     <row r="2" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" s="17"/>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="52"/>
+        <v>5</v>
+      </c>
+      <c r="B9" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="55"/>
       <c r="H9" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
@@ -1564,65 +1711,65 @@
         <v>#VALUE!</v>
       </c>
       <c r="I10" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J10" s="37" t="e">
         <f>H10/I10</f>
         <v>#VALUE!</v>
       </c>
       <c r="K10" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D11" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="F11" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="G11" s="29" t="s">
         <v>73</v>
-      </c>
-      <c r="G11" s="29" t="s">
-        <v>74</v>
       </c>
       <c r="H11" s="28" t="e">
         <f>24*((D11-E11)-(B11-C11))/(F11*G11*D16)</f>
         <v>#VALUE!</v>
       </c>
       <c r="I11" s="30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J11" s="37" t="e">
         <f t="shared" ref="J11:J12" si="0">H11/I11</f>
         <v>#VALUE!</v>
       </c>
       <c r="K11" s="30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E12" s="28"/>
       <c r="F12" s="28"/>
@@ -1632,30 +1779,30 @@
         <v>#VALUE!</v>
       </c>
       <c r="I12" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J12" s="37" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="K12" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="21"/>
@@ -1664,13 +1811,13 @@
     </row>
     <row r="15" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
@@ -1679,176 +1826,176 @@
     </row>
     <row r="16" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" s="21"/>
     </row>
     <row r="17" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" s="21"/>
     </row>
     <row r="18" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:11" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" s="53" t="s">
-        <v>79</v>
-      </c>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54"/>
-      <c r="E26" s="54"/>
-      <c r="F26" s="54"/>
-      <c r="G26" s="54"/>
-      <c r="H26" s="54"/>
-      <c r="I26" s="54"/>
-      <c r="J26" s="55"/>
+      <c r="A26" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="57"/>
+      <c r="J26" s="58"/>
       <c r="K26" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="39"/>
-      <c r="B27" s="56"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="57"/>
-      <c r="G27" s="57"/>
-      <c r="H27" s="57"/>
-      <c r="I27" s="57"/>
-      <c r="J27" s="58"/>
+      <c r="A27" s="42"/>
+      <c r="B27" s="59"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="60"/>
+      <c r="I27" s="60"/>
+      <c r="J27" s="61"/>
       <c r="K27" s="33" t="e">
         <f>((J10^K10)*(J11^K11)*(J12^K12))^(1/3)</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="39"/>
-      <c r="B28" s="56"/>
-      <c r="C28" s="57"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="57"/>
-      <c r="H28" s="57"/>
-      <c r="I28" s="57"/>
-      <c r="J28" s="58"/>
+      <c r="A28" s="42"/>
+      <c r="B28" s="59"/>
+      <c r="C28" s="60"/>
+      <c r="D28" s="60"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="60"/>
+      <c r="H28" s="60"/>
+      <c r="I28" s="60"/>
+      <c r="J28" s="61"/>
     </row>
     <row r="29" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="39"/>
-      <c r="B29" s="56"/>
-      <c r="C29" s="57"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="57"/>
-      <c r="H29" s="57"/>
-      <c r="I29" s="57"/>
-      <c r="J29" s="58"/>
+      <c r="A29" s="42"/>
+      <c r="B29" s="59"/>
+      <c r="C29" s="60"/>
+      <c r="D29" s="60"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="60"/>
+      <c r="H29" s="60"/>
+      <c r="I29" s="60"/>
+      <c r="J29" s="61"/>
     </row>
     <row r="30" spans="1:11" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="40"/>
-      <c r="B30" s="59"/>
-      <c r="C30" s="60"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="60"/>
-      <c r="H30" s="60"/>
-      <c r="I30" s="60"/>
-      <c r="J30" s="61"/>
+      <c r="A30" s="43"/>
+      <c r="B30" s="62"/>
+      <c r="C30" s="63"/>
+      <c r="D30" s="63"/>
+      <c r="E30" s="63"/>
+      <c r="F30" s="63"/>
+      <c r="G30" s="63"/>
+      <c r="H30" s="63"/>
+      <c r="I30" s="63"/>
+      <c r="J30" s="64"/>
     </row>
     <row r="31" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="24"/>
@@ -1864,12 +2011,12 @@
     <row r="32" spans="1:11" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1884,31 +2031,525 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E76612D3-D564-4DFB-98A8-81EE36785683}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D38B1E9F-2C5A-4D5A-AD7A-8DA28964D438}">
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="79.83203125" style="2" customWidth="1"/>
+    <col min="2" max="5" width="16.83203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="28.83203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="27.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="30" style="2" customWidth="1"/>
+    <col min="9" max="9" width="23.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.5" style="2" customWidth="1"/>
+    <col min="11" max="11" width="18.5" style="2" customWidth="1"/>
+    <col min="12" max="12" width="15.1640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="9.1640625" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="31" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="5"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="5"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:9" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="28" t="str">
+        <f>B8</f>
+        <v>ввод ЭД</v>
+      </c>
+      <c r="G8" s="28" t="str">
+        <f>Водозащита!F8</f>
+        <v>ввод ЭД</v>
+      </c>
+      <c r="H8" s="26" t="e">
+        <f>F8/G8</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="28" t="str">
+        <f>B9</f>
+        <v>ввод ЭД</v>
+      </c>
+      <c r="G9" s="28" t="str">
+        <f>Водозащита!F9</f>
+        <v>ввод ЭД</v>
+      </c>
+      <c r="H9" s="26" t="e">
+        <f t="shared" ref="H9:H12" si="0">F9/G9</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I9" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="28" t="str">
+        <f>B10</f>
+        <v>ввод ЭД</v>
+      </c>
+      <c r="G10" s="28" t="str">
+        <f>Водозащита!F10</f>
+        <v>ввод ЭД</v>
+      </c>
+      <c r="H10" s="26" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I10" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="35" t="e">
+        <f>1-((0.25*(B17-C11)+B11)/(0.25*B17))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G11" s="35" t="e">
+        <f>Водозащита!F11</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H11" s="26" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I11" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="28" t="str">
+        <f>B9</f>
+        <v>ввод ЭД</v>
+      </c>
+      <c r="C12" s="33" t="str">
+        <f>Водозащита!B9</f>
+        <v>ввод ЭД</v>
+      </c>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12" s="35" t="e">
+        <f>(C12-B12)/B18</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="26" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I12" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="65" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" s="66"/>
+      <c r="D19" s="65" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19" s="66"/>
+      <c r="F19" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="H19" s="65" t="s">
+        <v>103</v>
+      </c>
+      <c r="I19" s="67"/>
+      <c r="J19" s="66"/>
+    </row>
+    <row r="20" spans="1:10" ht="43" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="69"/>
+      <c r="D20" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="69"/>
+      <c r="F20" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="G20" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="H20" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="I20" s="71"/>
+      <c r="J20" s="69"/>
+    </row>
+    <row r="21" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="72" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" s="72" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="49" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="42"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="73" t="e">
+        <f>((H8^I8)*(H9^I9)*(H10^I10)*(H11^I11)*(H12^I12))^(1/5)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="42"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="49"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="42"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="49"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="42"/>
+      <c r="B27" s="47"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="49"/>
+    </row>
+    <row r="28" spans="1:10" ht="49" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="43"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="52"/>
+    </row>
+    <row r="29" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:10" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="17"/>
+    </row>
+    <row r="31" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="B23:H28"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="H20:J20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC5646C8-284D-41CD-9523-4B77C14C8468}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="118" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="50" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:2" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="38"/>
+      <c r="B4" s="74"/>
+    </row>
+    <row r="5" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="38"/>
+      <c r="B5" s="74"/>
+    </row>
+    <row r="6" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="38"/>
+      <c r="B6" s="74"/>
+    </row>
+    <row r="7" spans="1:2" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="38"/>
+      <c r="B7" s="74"/>
+    </row>
+    <row r="8" spans="1:2" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="75" t="e">
+        <f>(B1*Водозащита!I19)+(B2*Гомеостаз!K27)+(B3*Надежность!I24)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="38"/>
+      <c r="B9" s="74"/>
+    </row>
+    <row r="10" spans="1:2" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" s="75" t="e">
+        <f>((Водозащита!I19^B1)*(Гомеостаз!K27^B2)*(Надежность!I24^B3))^(1/3)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
create layers bugfixes, wrap material creation into a transaction
</commit_message>
<xml_diff>
--- a/static/exel_templates/report_template.xlsx
+++ b/static/exel_templates/report_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniil/Desktop/DIPLOM/evaluatingMaterialApp/static/exel_templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniil/Desktop/UNIVER/DIPLOM/evaluatingMaterialApp/static/exel_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58126F11-0663-1F4B-837D-343FBAA385F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264D58AC-BB04-BB4B-AF0E-D83E2E8F3FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="2" xr2:uid="{EDD4186A-6E89-4516-944D-5EFD2E0820A6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{EDD4186A-6E89-4516-944D-5EFD2E0820A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Водозащита" sheetId="1" r:id="rId1"/>
@@ -1287,7 +1287,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView zoomScale="93" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -1642,8 +1642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA1B50F2-689A-48B0-86F9-2E2A4FD4E6ED}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView zoomScale="81" zoomScaleNormal="119" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="119" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -2073,8 +2073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D38B1E9F-2C5A-4D5A-AD7A-8DA28964D438}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView zoomScale="83" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -2273,7 +2273,7 @@
       </c>
       <c r="D12"/>
       <c r="F12" s="35" t="e">
-        <f>B13/((C12-B12)/B18)</f>
+        <f>B14/((C12-B12)/B18)</f>
         <v>#VALUE!</v>
       </c>
       <c r="G12" s="28" t="s">
@@ -2288,21 +2288,21 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="46" t="s">
+      <c r="A13" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="B13" s="48" t="s">
+      <c r="B14" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="47" t="s">
+      <c r="C14" s="47" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="6"/>
     </row>
     <row r="15" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">

</xml_diff>